<commit_message>
Updated 040625-skills.xlsx with latest changes
</commit_message>
<xml_diff>
--- a/040625-skills.xlsx
+++ b/040625-skills.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github-sdooley-dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\629459\Documents\_ career\sdooley-dev.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0682C3C1-DB37-4563-A315-3D1E7820837A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8AC614-2BEC-4E43-A0C5-E50E35ABC2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45168" yWindow="912" windowWidth="34560" windowHeight="18552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="124">
   <si>
     <t>e_id</t>
   </si>
@@ -450,6 +450,15 @@
   </si>
   <si>
     <t>Selenium</t>
+  </si>
+  <si>
+    <t>06- Workshops, Bootcamps and Presentations</t>
+  </si>
+  <si>
+    <t>Agentic AI Innovation Session with AWS and Salesforce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agentic AI products are revolutionizing the tech landscape. Clients can use Agentic AI to deploy a digital workforce,  enhancing their workflows with efficiency and speed.  AWS and Salesforce explore  their Agentic AI products and perform a demo of a  use case Salesforce built for DOGE.  This is an ideation session for Booz Allen technical  and sales leader for use cases we can  co-develop and close with our partners. </t>
   </si>
 </sst>
 </file>
@@ -528,9 +537,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -542,6 +548,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,33 +769,33 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="12.5703125" style="7"/>
-    <col min="5" max="5" width="31.7109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="7"/>
+    <col min="5" max="5" width="31.7265625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -829,7 +838,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25">
+    <row r="2" spans="1:26" ht="14">
       <c r="A2" s="3">
         <v>16</v>
       </c>
@@ -842,7 +851,7 @@
       <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="4"/>
@@ -859,15 +868,15 @@
       <c r="M2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25">
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+    </row>
+    <row r="3" spans="1:26" ht="14">
       <c r="A3" s="3">
         <v>8</v>
       </c>
@@ -880,10 +889,10 @@
       <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="4" t="s">
         <v>24</v>
       </c>
@@ -893,23 +902,23 @@
       <c r="I3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="9"/>
+      <c r="K3" s="16"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-    </row>
-    <row r="4" spans="1:26" ht="14.25">
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+    </row>
+    <row r="4" spans="1:26" ht="14">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -922,7 +931,7 @@
       <c r="D4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="12" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="3">
@@ -934,22 +943,22 @@
       <c r="H4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="9"/>
+      <c r="N4" s="16"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="14.25">
+    <row r="5" spans="1:26" ht="14">
       <c r="A5" s="3">
         <v>13</v>
       </c>
@@ -962,7 +971,7 @@
       <c r="D5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="4"/>
@@ -978,16 +987,16 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:26" ht="14.25">
+    <row r="6" spans="1:26" ht="14">
       <c r="A6" s="3">
         <v>14</v>
       </c>
@@ -997,33 +1006,33 @@
       <c r="C6" s="5">
         <v>44531</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="16"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-    </row>
-    <row r="7" spans="1:26" ht="14.25">
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+    </row>
+    <row r="7" spans="1:26" ht="14">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -1036,10 +1045,10 @@
       <c r="D7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="4" t="s">
         <v>46</v>
       </c>
@@ -1049,11 +1058,11 @@
       <c r="I7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
       <c r="M7" s="4" t="s">
         <v>28</v>
       </c>
@@ -1063,7 +1072,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:26" ht="14.25">
+    <row r="8" spans="1:26" ht="14">
       <c r="A8" s="3">
         <v>15</v>
       </c>
@@ -1073,11 +1082,11 @@
       <c r="C8" s="5">
         <v>44614</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1091,15 +1100,15 @@
       <c r="M8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25">
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+    </row>
+    <row r="9" spans="1:26" ht="14">
       <c r="A9" s="3">
         <v>17</v>
       </c>
@@ -1109,69 +1118,69 @@
       <c r="C9" s="5">
         <v>44795</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
       <c r="G9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="16"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="N9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25">
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+    </row>
+    <row r="10" spans="1:26" ht="14">
       <c r="A10" s="3">
         <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>45242</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="16"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="N10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.25">
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+    </row>
+    <row r="11" spans="1:26" ht="14">
       <c r="A11" s="3">
         <v>23</v>
       </c>
@@ -1181,69 +1190,69 @@
       <c r="C11" s="5">
         <v>44958</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="9"/>
+      <c r="I11" s="16"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25">
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+    </row>
+    <row r="12" spans="1:26" ht="14">
       <c r="A12" s="3">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>44911</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="9"/>
+      <c r="I12" s="16"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N12" s="10" t="s">
+      <c r="N12" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25">
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+    </row>
+    <row r="13" spans="1:26" ht="14">
       <c r="A13" s="3">
         <v>24</v>
       </c>
@@ -1253,33 +1262,33 @@
       <c r="C13" s="5">
         <v>44986</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
       <c r="G13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="N13" s="10" t="s">
+      <c r="N13" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25">
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+    </row>
+    <row r="14" spans="1:26" ht="14">
       <c r="A14" s="3">
         <v>25</v>
       </c>
@@ -1289,33 +1298,33 @@
       <c r="C14" s="5">
         <v>45078</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="N14" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25">
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+    </row>
+    <row r="15" spans="1:26" ht="14">
       <c r="A15" s="3">
         <v>26</v>
       </c>
@@ -1325,33 +1334,33 @@
       <c r="C15" s="5">
         <v>45047</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N15" s="10" t="s">
+      <c r="N15" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-    </row>
-    <row r="16" spans="1:26" ht="14.25">
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+    </row>
+    <row r="16" spans="1:26" ht="14">
       <c r="A16" s="3">
         <v>27</v>
       </c>
@@ -1361,31 +1370,31 @@
       <c r="C16" s="5">
         <v>45078</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="8" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N16" s="10" t="s">
+      <c r="N16" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-    </row>
-    <row r="17" spans="1:18" ht="14.25">
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+    </row>
+    <row r="17" spans="1:18" ht="14">
       <c r="A17" s="3">
         <v>28</v>
       </c>
@@ -1395,31 +1404,31 @@
       <c r="C17" s="5">
         <v>45078</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="8" t="s">
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N17" s="10" t="s">
+      <c r="N17" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-    </row>
-    <row r="18" spans="1:18" ht="14.25">
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+    </row>
+    <row r="18" spans="1:18" ht="14">
       <c r="A18" s="3">
         <v>29</v>
       </c>
@@ -1429,15 +1438,15 @@
       <c r="C18" s="5">
         <v>45108</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="8" t="s">
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="9"/>
+      <c r="H18" s="16"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -1445,15 +1454,15 @@
       <c r="M18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="N18" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-    </row>
-    <row r="19" spans="1:18" ht="14.25">
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+    </row>
+    <row r="19" spans="1:18" ht="14">
       <c r="A19" s="3">
         <v>30</v>
       </c>
@@ -1463,15 +1472,15 @@
       <c r="C19" s="5">
         <v>45231</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="8" t="s">
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -1479,15 +1488,15 @@
       <c r="M19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-    </row>
-    <row r="20" spans="1:18" ht="14.25">
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+    </row>
+    <row r="20" spans="1:18" ht="14">
       <c r="A20" s="3">
         <v>31</v>
       </c>
@@ -1497,35 +1506,35 @@
       <c r="C20" s="5">
         <v>45292</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
       <c r="G20" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J20" s="9"/>
+      <c r="J20" s="16"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N20" s="10" t="s">
+      <c r="N20" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-    </row>
-    <row r="21" spans="1:18" ht="14.25">
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+    </row>
+    <row r="21" spans="1:18" ht="14">
       <c r="A21" s="3">
         <v>32</v>
       </c>
@@ -1535,10 +1544,10 @@
       <c r="C21" s="5">
         <v>45323</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="9"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4" t="s">
         <v>73</v>
@@ -1546,24 +1555,24 @@
       <c r="H21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J21" s="16"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N21" s="10" t="s">
+      <c r="N21" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-    </row>
-    <row r="22" spans="1:18" ht="14.25">
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+    </row>
+    <row r="22" spans="1:18" ht="14">
       <c r="A22" s="3">
         <v>33</v>
       </c>
@@ -1573,10 +1582,10 @@
       <c r="C22" s="5">
         <v>45323</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="9"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
         <v>73</v>
@@ -1584,24 +1593,24 @@
       <c r="H22" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="9"/>
+      <c r="J22" s="16"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="10" t="s">
+      <c r="N22" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-    </row>
-    <row r="23" spans="1:18" ht="14.25">
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+    </row>
+    <row r="23" spans="1:18" ht="14">
       <c r="A23" s="3">
         <v>34</v>
       </c>
@@ -1611,31 +1620,31 @@
       <c r="C23" s="5">
         <v>45292</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="8" t="s">
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N23" s="10" t="s">
+      <c r="N23" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-    </row>
-    <row r="24" spans="1:18" ht="14.25">
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+    </row>
+    <row r="24" spans="1:18" ht="14">
       <c r="A24" s="3">
         <v>35</v>
       </c>
@@ -1645,31 +1654,31 @@
       <c r="C24" s="5">
         <v>45261</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="8" t="s">
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N24" s="10" t="s">
+      <c r="N24" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-    </row>
-    <row r="25" spans="1:18" ht="14.25">
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+    </row>
+    <row r="25" spans="1:18" ht="14">
       <c r="A25" s="3">
         <v>36</v>
       </c>
@@ -1679,11 +1688,11 @@
       <c r="C25" s="5">
         <v>45627</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="4" t="s">
         <v>87</v>
       </c>
@@ -1699,15 +1708,15 @@
       <c r="M25" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N25" s="10" t="s">
+      <c r="N25" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-    </row>
-    <row r="26" spans="1:18" ht="14.25">
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+    </row>
+    <row r="26" spans="1:18" ht="14">
       <c r="A26" s="3">
         <v>38</v>
       </c>
@@ -1717,11 +1726,11 @@
       <c r="C26" s="5">
         <v>45689</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="4" t="s">
         <v>73</v>
       </c>
@@ -1732,16 +1741,16 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="8" t="s">
+      <c r="M26" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="N26" s="9"/>
+      <c r="N26" s="16"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" ht="14.25">
+    <row r="27" spans="1:18" ht="14">
       <c r="A27" s="3">
         <v>39</v>
       </c>
@@ -1751,33 +1760,33 @@
       <c r="C27" s="5">
         <v>45717</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="16"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="N27" s="10" t="s">
+      <c r="N27" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-    </row>
-    <row r="28" spans="1:18" ht="14.25">
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+    </row>
+    <row r="28" spans="1:18" ht="14">
       <c r="A28" s="3">
         <v>41</v>
       </c>
@@ -1787,11 +1796,11 @@
       <c r="C28" s="5">
         <v>45717</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="4" t="s">
         <v>26</v>
       </c>
@@ -1813,7 +1822,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" ht="14.25">
+    <row r="29" spans="1:18" ht="14">
       <c r="A29" s="3">
         <v>40</v>
       </c>
@@ -1826,10 +1835,10 @@
       <c r="D29" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="F29" s="9"/>
+      <c r="F29" s="16"/>
       <c r="G29" s="4" t="s">
         <v>26</v>
       </c>
@@ -1845,15 +1854,15 @@
       <c r="M29" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="N29" s="10" t="s">
+      <c r="N29" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-    </row>
-    <row r="30" spans="1:18" ht="14.25">
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+    </row>
+    <row r="30" spans="1:18" ht="14">
       <c r="A30" s="3">
         <v>10</v>
       </c>
@@ -1866,7 +1875,7 @@
       <c r="D30" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="12" t="s">
         <v>105</v>
       </c>
       <c r="F30" s="4"/>
@@ -1880,16 +1889,16 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="8" t="s">
+      <c r="M30" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="14.25">
+    <row r="31" spans="1:18" ht="14">
       <c r="A31" s="3">
         <v>11</v>
       </c>
@@ -1902,7 +1911,7 @@
       <c r="D31" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="12" t="s">
         <v>110</v>
       </c>
       <c r="F31" s="4"/>
@@ -1916,16 +1925,16 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="8" t="s">
+      <c r="M31" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="N31" s="9"/>
+      <c r="N31" s="16"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="14.25">
+    <row r="32" spans="1:18" ht="14">
       <c r="A32" s="3">
         <v>12</v>
       </c>
@@ -1938,7 +1947,7 @@
       <c r="D32" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="12" t="s">
         <v>114</v>
       </c>
       <c r="F32" s="4"/>
@@ -1952,12 +1961,12 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="8" t="s">
+      <c r="M32" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
@@ -1974,7 +1983,7 @@
       <c r="D33" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="13" t="s">
         <v>119</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -1987,69 +1996,40 @@
         <v>120</v>
       </c>
     </row>
+    <row r="34" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A34" s="3">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="7">
+        <v>45776</v>
+      </c>
+      <c r="D34" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" t="s">
+        <v>24</v>
+      </c>
+      <c r="J34" t="s">
+        <v>41</v>
+      </c>
+      <c r="M34" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="N12:R12"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="N10:R10"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="N13:R13"/>
-    <mergeCell ref="N14:R14"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="N16:R16"/>
-    <mergeCell ref="N17:R17"/>
     <mergeCell ref="M31:N31"/>
     <mergeCell ref="M32:P32"/>
     <mergeCell ref="N18:R18"/>
@@ -2064,6 +2044,67 @@
     <mergeCell ref="N27:R27"/>
     <mergeCell ref="N29:R29"/>
     <mergeCell ref="M30:P30"/>
+    <mergeCell ref="N13:R13"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="N15:R15"/>
+    <mergeCell ref="N16:R16"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="N12:R12"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="N10:R10"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="I21:J21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2092,4 +2133,10 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{3de9faa6-9fe1-49b3-9a08-227a296b54a6}" enabled="1" method="Privileged" siteId="{d5fe813e-0caa-432a-b2ac-d555aa91bd1c}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update 040625-skills.xlsx - uploaded via Claude Opus 4.6 workflow - February 16, 2026 at 06:07 PM
</commit_message>
<xml_diff>
--- a/040625-skills.xlsx
+++ b/040625-skills.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\claude_projects\sd_github_021626\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EB0C6D-51F1-4828-918D-19C7B2F97240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C16EE0-96C1-4AB1-8A88-ABF4A675F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45456" yWindow="624" windowWidth="34560" windowHeight="18648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="214">
   <si>
     <t>e_id</t>
   </si>
@@ -697,9 +697,6 @@
     <t>Technical Certifications</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Gold Award</t>
   </si>
   <si>
@@ -746,6 +743,18 @@
   </si>
   <si>
     <t>Moveworks/ServiceNow Agentic AI Workflow</t>
+  </si>
+  <si>
+    <t>yaml</t>
+  </si>
+  <si>
+    <t>claude code</t>
+  </si>
+  <si>
+    <t>github</t>
+  </si>
+  <si>
+    <t>Claude Code - GitHub Deployment Workflow</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1176,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D75" sqref="D75"/>
+      <selection pane="bottomRight" activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3600,7 +3609,7 @@
         <v>45678</v>
       </c>
       <c r="D62" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E62" s="23" t="s">
         <v>138</v>
@@ -3635,7 +3644,7 @@
         <v>45645</v>
       </c>
       <c r="D63" s="34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E63" s="23" t="s">
         <v>138</v>
@@ -3664,7 +3673,7 @@
         <v>45534</v>
       </c>
       <c r="D64" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E64" s="23" t="s">
         <v>138</v>
@@ -3693,7 +3702,7 @@
         <v>45467</v>
       </c>
       <c r="D65" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E65" s="23" t="s">
         <v>138</v>
@@ -3722,7 +3731,7 @@
         <v>44973</v>
       </c>
       <c r="D66" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E66" s="23" t="s">
         <v>138</v>
@@ -3751,7 +3760,7 @@
         <v>45930</v>
       </c>
       <c r="D67" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E67" s="23" t="s">
         <v>138</v>
@@ -3780,7 +3789,7 @@
         <v>45930</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E68" s="23" t="s">
         <v>138</v>
@@ -3809,7 +3818,7 @@
         <v>45930</v>
       </c>
       <c r="D69" s="34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E69" s="35" t="s">
         <v>138</v>
@@ -3818,7 +3827,7 @@
       <c r="I69"/>
       <c r="J69"/>
       <c r="M69" s="22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P69" t="s">
         <v>128</v>
@@ -3838,7 +3847,7 @@
         <v>45930</v>
       </c>
       <c r="D70" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E70" s="35" t="s">
         <v>138</v>
@@ -3847,7 +3856,7 @@
       <c r="I70"/>
       <c r="J70"/>
       <c r="M70" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P70" t="s">
         <v>128</v>
@@ -3867,7 +3876,7 @@
         <v>45998</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E71" s="35" t="s">
         <v>138</v>
@@ -3878,7 +3887,7 @@
       <c r="I71"/>
       <c r="J71"/>
       <c r="M71" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P71" t="s">
         <v>129</v>
@@ -3898,21 +3907,23 @@
         <v>46066</v>
       </c>
       <c r="D72" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="E72" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="G72" t="s">
+        <v>206</v>
+      </c>
+      <c r="H72" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="I72" t="s">
+        <v>208</v>
+      </c>
+      <c r="J72" t="s">
         <v>210</v>
       </c>
-      <c r="E72" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="G72" t="s">
-        <v>207</v>
-      </c>
-      <c r="H72" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="I72" t="s">
-        <v>209</v>
-      </c>
-      <c r="J72"/>
       <c r="M72" s="19" t="s">
         <v>59</v>
       </c>
@@ -3925,11 +3936,37 @@
     </row>
     <row r="73" spans="1:17" ht="15.75" customHeight="1">
       <c r="A73" s="3">
-        <v>999</v>
-      </c>
-      <c r="B73" s="8"/>
+        <v>83</v>
+      </c>
+      <c r="B73" t="s">
+        <v>121</v>
+      </c>
+      <c r="C73" s="12">
+        <v>46069</v>
+      </c>
       <c r="D73" s="14" t="s">
-        <v>194</v>
+        <v>213</v>
+      </c>
+      <c r="E73" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="G73" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="H73" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="I73" t="s">
+        <v>206</v>
+      </c>
+      <c r="M73" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="P73" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3937,7 +3974,7 @@
     <sortCondition ref="A2:A42"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:B39 B41 B32:B34 B2:B28 B61:B70 B73" xr:uid="{ED44EAAA-DACA-40E8-A7DB-D96063B10E1E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:B39 B41 B32:B34 B2:B28 B61:B70" xr:uid="{ED44EAAA-DACA-40E8-A7DB-D96063B10E1E}">
       <formula1>$T$3:$T$8</formula1>
     </dataValidation>
   </dataValidations>
@@ -3962,7 +3999,7 @@
     <hyperlink ref="N9" r:id="rId18" xr:uid="{0B930030-61CB-4F57-8E2F-66C14A1FF8B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId19"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId19"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
Update 040625-skills.xlsx - uploaded via Claude Opus 4.6 workflow - February 16, 2026 at 06:17 PM
</commit_message>
<xml_diff>
--- a/040625-skills.xlsx
+++ b/040625-skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\claude_projects\sd_github_021626\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C16EE0-96C1-4AB1-8A88-ABF4A675F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E2E2B4-D3DE-4FEE-AD42-4E44A1D6C429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="212">
   <si>
     <t>e_id</t>
   </si>
@@ -725,12 +725,6 @@
   </si>
   <si>
     <t>Awards</t>
-  </si>
-  <si>
-    <t>Ai and the Future of Productivity</t>
-  </si>
-  <si>
-    <t>OpenAI</t>
   </si>
   <si>
     <t>agentic ai</t>
@@ -1170,13 +1164,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z73"/>
+  <dimension ref="A1:Z72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I81" sqref="I81"/>
+      <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3867,27 +3861,34 @@
     </row>
     <row r="71" spans="1:17" ht="15.75" customHeight="1">
       <c r="A71" s="3">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="C71" s="12">
-        <v>45998</v>
+        <v>46066</v>
       </c>
       <c r="D71" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="E71" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="G71" t="s">
         <v>204</v>
       </c>
-      <c r="E71" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="G71" t="s">
-        <v>24</v>
-      </c>
-      <c r="I71"/>
-      <c r="J71"/>
-      <c r="M71" s="22" t="s">
+      <c r="H71" s="19" t="s">
         <v>205</v>
+      </c>
+      <c r="I71" t="s">
+        <v>206</v>
+      </c>
+      <c r="J71" t="s">
+        <v>208</v>
+      </c>
+      <c r="M71" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="P71" t="s">
         <v>129</v>
@@ -3898,31 +3899,28 @@
     </row>
     <row r="72" spans="1:17" ht="15.75" customHeight="1">
       <c r="A72" s="3">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B72" t="s">
         <v>121</v>
       </c>
       <c r="C72" s="12">
-        <v>46066</v>
-      </c>
-      <c r="D72" s="34" t="s">
+        <v>46069</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="E72" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="G72" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="E72" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="G72" t="s">
-        <v>206</v>
-      </c>
       <c r="H72" s="19" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="I72" t="s">
-        <v>208</v>
-      </c>
-      <c r="J72" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="M72" s="19" t="s">
         <v>59</v>
@@ -3931,41 +3929,6 @@
         <v>129</v>
       </c>
       <c r="Q72" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A73" s="3">
-        <v>83</v>
-      </c>
-      <c r="B73" t="s">
-        <v>121</v>
-      </c>
-      <c r="C73" s="12">
-        <v>46069</v>
-      </c>
-      <c r="D73" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="E73" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="G73" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="H73" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="I73" t="s">
-        <v>206</v>
-      </c>
-      <c r="M73" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="P73" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q73" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update 040625-skills.xlsx - uploaded via Claude Opus 4.6 workflow - February 16, 2026 at 06:23 PM
</commit_message>
<xml_diff>
--- a/040625-skills.xlsx
+++ b/040625-skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\claude_projects\sd_github_021626\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E2E2B4-D3DE-4FEE-AD42-4E44A1D6C429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A16110-ACBB-4DBD-B044-AC8D9B16C0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="212">
   <si>
     <t>e_id</t>
   </si>
@@ -1167,10 +1167,10 @@
   <dimension ref="A1:Z72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
+      <selection pane="bottomRight" activeCell="Q74" sqref="Q74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3295,9 +3295,6 @@
       <c r="R54">
         <v>2</v>
       </c>
-      <c r="S54" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="55" spans="1:19" ht="15.75" customHeight="1">
       <c r="A55" s="3">
@@ -3338,9 +3335,6 @@
       </c>
       <c r="R55">
         <v>2</v>
-      </c>
-      <c r="S55" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:19" ht="15.75" customHeight="1">
@@ -3685,7 +3679,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="15.75" customHeight="1">
+    <row r="65" spans="1:19" ht="15.75" customHeight="1">
       <c r="A65" s="3">
         <v>75</v>
       </c>
@@ -3714,7 +3708,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="15.75" customHeight="1">
+    <row r="66" spans="1:19" ht="15.75" customHeight="1">
       <c r="A66" s="3">
         <v>76</v>
       </c>
@@ -3743,7 +3737,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="15.75" customHeight="1">
+    <row r="67" spans="1:19" ht="15.75" customHeight="1">
       <c r="A67" s="3">
         <v>77</v>
       </c>
@@ -3771,8 +3765,14 @@
       <c r="Q67" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" ht="15.75" customHeight="1">
+      <c r="R67">
+        <v>1</v>
+      </c>
+      <c r="S67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="15.75" customHeight="1">
       <c r="A68" s="3">
         <v>78</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="15.75" customHeight="1">
+    <row r="69" spans="1:19" ht="15.75" customHeight="1">
       <c r="A69" s="3">
         <v>79</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="15.75" customHeight="1">
+    <row r="70" spans="1:19" ht="15.75" customHeight="1">
       <c r="A70" s="3">
         <v>80</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="15.75" customHeight="1">
+    <row r="71" spans="1:19" ht="15.75" customHeight="1">
       <c r="A71" s="3">
         <v>82</v>
       </c>
@@ -3896,8 +3896,14 @@
       <c r="Q71" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" ht="15.75" customHeight="1">
+      <c r="R71">
+        <v>2</v>
+      </c>
+      <c r="S71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" ht="15.75" customHeight="1">
       <c r="A72" s="3">
         <v>83</v>
       </c>
@@ -3930,6 +3936,12 @@
       </c>
       <c r="Q72" t="s">
         <v>129</v>
+      </c>
+      <c r="R72">
+        <v>1</v>
+      </c>
+      <c r="S72" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>